<commit_message>
Update data and analysis files
- Edit mistakes in file names of existing data files
- Add filenames files for GUIDEseq experiments
- Add SRA filename outputs from analysis
- Add Fig 6a and Fig S1a images to repository
- Changed analysis code to output source data files
  and file descriptions for SRA submission
</commit_message>
<xml_diff>
--- a/Stat_analysis/source_data_file.xlsx
+++ b/Stat_analysis/source_data_file.xlsx
@@ -14133,7 +14133,7 @@
         <v>24</v>
       </c>
       <c r="E2" t="n">
-        <v>0.082236842</v>
+        <v>0.002529148</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -14153,7 +14153,7 @@
         <v>24</v>
       </c>
       <c r="E3" t="n">
-        <v>0.132383534</v>
+        <v>0.00351413</v>
       </c>
       <c r="F3" t="n">
         <v>0.002363899</v>
@@ -14173,7 +14173,7 @@
         <v>24</v>
       </c>
       <c r="E4" t="n">
-        <v>0.070422535</v>
+        <v>0.001559916</v>
       </c>
       <c r="F4" t="n">
         <v>0.002589399</v>
@@ -14465,7 +14465,7 @@
         <v>24</v>
       </c>
       <c r="E2" t="n">
-        <v>0.082236842</v>
+        <v>0.002529148</v>
       </c>
       <c r="F2"/>
     </row>
@@ -14483,7 +14483,7 @@
         <v>24</v>
       </c>
       <c r="E3" t="n">
-        <v>0.132383534</v>
+        <v>0.00351413</v>
       </c>
       <c r="F3" t="n">
         <v>0.049682708</v>
@@ -14503,7 +14503,7 @@
         <v>24</v>
       </c>
       <c r="E4" t="n">
-        <v>0.070422535</v>
+        <v>0.001559916</v>
       </c>
       <c r="F4" t="n">
         <v>0.026878108</v>

</xml_diff>